<commit_message>
Avance inicio de sesión + creación de noticia
</commit_message>
<xml_diff>
--- a/docs/iso25010.xlsx
+++ b/docs/iso25010.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SHAIR\home\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SHAIR\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC80359-EA54-435E-B989-7E2DBB868C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E025AC-FB27-4C38-9246-53D929E6076B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1191,7 +1191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1205,61 +1205,80 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
-      <name val="Arial"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Arial"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5E0B3"/>
-        <bgColor rgb="FFC5E0B3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFD9"/>
-        <bgColor rgb="FFE2EFD9"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1319,6 +1338,36 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF2E75B5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor rgb="FFFFD965"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor rgb="FFC5E0B3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
   </fills>
@@ -1537,7 +1586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1548,40 +1597,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1590,142 +1681,121 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1770,9 +1840,9 @@
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -1780,8 +1850,9 @@
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Cumplimiento de Expectativas De Proyecto</a:t>
             </a:r>
@@ -1805,9 +1876,9 @@
               <a:solidFill>
                 <a:srgbClr val="757575"/>
               </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="es-CO"/>
@@ -1897,8 +1968,8 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -1985,7 +2056,7 @@
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
@@ -2044,8 +2115,9 @@
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -2053,8 +2125,9 @@
                 <a:solidFill>
                   <a:srgbClr val="757575"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="34" charset="0"/>
               </a:rPr>
               <a:t>Gráfico De Notas Cuantitativas Del Proyecto</a:t>
             </a:r>
@@ -2180,8 +2253,9 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-CO"/>
@@ -2246,8 +2320,9 @@
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="es-CO"/>
@@ -2300,7 +2375,8 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
@@ -2316,8 +2392,8 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
@@ -2333,8 +2409,8 @@
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
@@ -2428,8 +2504,9 @@
               <a:solidFill>
                 <a:srgbClr val="1A1A1A"/>
               </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="es-CO"/>
@@ -3293,9 +3370,9 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="5.7109375" style="4" customWidth="1"/>
     <col min="5" max="9" width="8.5703125" style="4" customWidth="1"/>
@@ -3308,7 +3385,7 @@
     <col min="24" max="25" width="10" style="4" customWidth="1"/>
     <col min="26" max="26" width="9.85546875" style="4" customWidth="1"/>
     <col min="27" max="27" width="10" style="4" customWidth="1"/>
-    <col min="28" max="28" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="4.7109375" style="4" customWidth="1"/>
     <col min="31" max="31" width="12.85546875" style="4" customWidth="1"/>
     <col min="32" max="32" width="3.85546875" style="4" customWidth="1"/>
@@ -3316,1623 +3393,1635 @@
     <col min="38" max="16384" width="14.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="16"/>
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
-    </row>
-    <row r="2" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="65"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="36" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="36" t="s">
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="32"/>
-      <c r="O2" s="43" t="s">
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="67"/>
+      <c r="O2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="45"/>
-      <c r="R2" s="60" t="s">
+      <c r="P2" s="33"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="62"/>
-      <c r="X2" s="18" t="s">
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="17"/>
-    </row>
-    <row r="3" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="37" t="s">
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="33"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="37">
+      <c r="E3" s="19">
         <v>1</v>
       </c>
-      <c r="F3" s="37">
+      <c r="F3" s="19">
         <v>2</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="19">
         <v>3</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="19">
         <v>4</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="19">
         <v>5</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="O3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="57" t="s">
+      <c r="P3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="63">
+      <c r="R3" s="20">
         <v>1</v>
       </c>
-      <c r="S3" s="63">
+      <c r="S3" s="20">
         <v>2</v>
       </c>
-      <c r="T3" s="63">
+      <c r="T3" s="20">
         <v>3</v>
       </c>
-      <c r="U3" s="63">
+      <c r="U3" s="20">
         <v>4</v>
       </c>
-      <c r="V3" s="63">
+      <c r="V3" s="20">
         <v>5</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="Y3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AA3" s="22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
         <v>1</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="19">
         <f t="shared" ref="C4:M4" si="0">COUNTA(C5:C7)</f>
         <v>3</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="37">
+      <c r="E4" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F4" s="37">
+      <c r="F4" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="19">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I4" s="37">
+      <c r="I4" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J4" s="37">
+      <c r="J4" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K4" s="37">
+      <c r="K4" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L4" s="37">
+      <c r="L4" s="19">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="M4" s="37">
+      <c r="M4" s="19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O4" s="57">
+      <c r="O4" s="5">
         <f t="shared" ref="O4:P4" si="1">(C4+C9+C14+C18+C26+C32+C39+C46)</f>
         <v>30</v>
       </c>
-      <c r="P4" s="57">
+      <c r="P4" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="R4" s="59">
+      <c r="R4" s="21">
         <f t="shared" ref="R4:V4" si="2">(E4+E9+E14+E18+E26+E32+E39+E46)</f>
         <v>1</v>
       </c>
-      <c r="S4" s="59">
+      <c r="S4" s="21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="T4" s="59">
+      <c r="T4" s="21">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="U4" s="59">
+      <c r="U4" s="21">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="V4" s="59">
+      <c r="V4" s="21">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="X4" s="5">
+      <c r="X4" s="22">
         <f t="shared" ref="X4:AA4" si="3">(J4+J9+J14+J18+J26+J32+J39+J46)</f>
         <v>1</v>
       </c>
-      <c r="Y4" s="5">
+      <c r="Y4" s="22">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="Z4" s="5">
+      <c r="Z4" s="22">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="AA4" s="5">
+      <c r="AA4" s="22">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="AF4" s="11"/>
+      <c r="AF4" s="7"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I5" s="59"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="M5" s="40"/>
-      <c r="AF5" s="11"/>
+      <c r="C5" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M5" s="10"/>
+      <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF6" s="11"/>
+      <c r="C6" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I7" s="59"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="M7" s="40"/>
-      <c r="AF7" s="11"/>
-    </row>
-    <row r="8" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="41"/>
-      <c r="O8" s="14" t="s">
+      <c r="C7" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="13"/>
+      <c r="O8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="28" t="s">
+      <c r="P8" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="28" t="s">
+      <c r="Q8" s="60"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="61"/>
+      <c r="T8" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="17"/>
-      <c r="Y8" s="15" t="s">
+      <c r="U8" s="60"/>
+      <c r="V8" s="60"/>
+      <c r="W8" s="61"/>
+      <c r="Y8" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="17"/>
-      <c r="AF8" s="11"/>
-    </row>
-    <row r="9" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="60"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="60"/>
+      <c r="AE8" s="61"/>
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
         <v>2</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="15">
         <f t="shared" ref="C9:M9" si="4">COUNTA(C10:C12)</f>
         <v>3</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="15">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="15">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="15">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L9" s="37">
+      <c r="L9" s="15">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M9" s="37">
+      <c r="M9" s="15">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="O9" s="12"/>
-      <c r="P9" s="19">
+      <c r="O9" s="27"/>
+      <c r="P9" s="37">
         <f>COUNTA(C5,C7,C12,C10,C16,C19,C23,C22,C42,C40,C44,C34,C33,C36,C27,C29,C47,C48,C30)</f>
         <v>19</v>
       </c>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="19">
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="37">
         <f>COUNTA(D7,D6,D10,D12,D15,D23,D20,D21,D40,D41,D35,D29,D47)</f>
         <v>1</v>
       </c>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="21"/>
-      <c r="Y9" s="15" t="s">
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="39"/>
+      <c r="Y9" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="Z9" s="17"/>
-      <c r="AA9" s="9">
+      <c r="Z9" s="33"/>
+      <c r="AA9" s="17">
         <f>(P9+P15)</f>
         <v>30</v>
       </c>
-      <c r="AB9" s="10">
+      <c r="AB9" s="18">
         <f>(P9+P15)/21</f>
         <v>1.4285714285714286</v>
       </c>
-      <c r="AC9" s="15" t="str">
+      <c r="AC9" s="29" t="str">
         <f>IF(AA9&gt;= 15, "Muy Prometedor","Evaluar Potencial")</f>
         <v>Muy Prometedor</v>
       </c>
-      <c r="AD9" s="16"/>
-      <c r="AE9" s="17"/>
-      <c r="AF9" s="11"/>
-    </row>
-    <row r="10" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="39" t="s">
+      <c r="AD9" s="30"/>
+      <c r="AE9" s="31"/>
+      <c r="AF9" s="7"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="O10" s="12"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="24"/>
-      <c r="Y10" s="15" t="s">
+      <c r="C10" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="O10" s="27"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="42"/>
+      <c r="Y10" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="Z10" s="17"/>
-      <c r="AA10" s="9">
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="17">
         <f>(T9+T15)</f>
         <v>1</v>
       </c>
-      <c r="AB10" s="10">
+      <c r="AB10" s="18">
         <f>(T9+T15)/21</f>
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="AC10" s="15" t="str">
+      <c r="AC10" s="29" t="str">
         <f>IF(Y10&gt;= 15,"Advertencia","Corregir Limites")</f>
         <v>Advertencia</v>
       </c>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="17"/>
-      <c r="AF10" s="11"/>
-    </row>
-    <row r="11" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39" t="s">
+      <c r="AD10" s="30"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I11" s="59"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="O11" s="12"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="24"/>
-      <c r="Y11" s="15" t="s">
+      <c r="C11" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="O11" s="27"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="42"/>
+      <c r="Y11" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="9">
+      <c r="Z11" s="33"/>
+      <c r="AA11" s="17">
         <f>(P9+T15)</f>
         <v>19</v>
       </c>
-      <c r="AB11" s="10">
+      <c r="AB11" s="18">
         <f>(P9+T15)/21</f>
         <v>0.90476190476190477</v>
       </c>
-      <c r="AC11" s="15" t="str">
+      <c r="AC11" s="29" t="str">
         <f>IF(AA11&lt;=15,"Que Tan Viable","Mucho Riesgo")</f>
         <v>Mucho Riesgo</v>
       </c>
-      <c r="AD11" s="16"/>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="11"/>
-    </row>
-    <row r="12" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="39" t="s">
+      <c r="AD11" s="30"/>
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="7"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="24"/>
-      <c r="Y12" s="15" t="s">
+      <c r="C12" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="42"/>
+      <c r="Y12" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="Z12" s="17"/>
-      <c r="AA12" s="9">
+      <c r="Z12" s="33"/>
+      <c r="AA12" s="17">
         <f>(T9+P15)</f>
         <v>12</v>
       </c>
-      <c r="AB12" s="10">
+      <c r="AB12" s="18">
         <f>(T9+P15)/21</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="AC12" s="15" t="str">
+      <c r="AC12" s="29" t="str">
         <f>IF(AA12&lt;=15,"Retos Por Enfrentar","Muchos Retos")</f>
         <v>Retos Por Enfrentar</v>
       </c>
-      <c r="AD12" s="16"/>
-      <c r="AE12" s="17"/>
-      <c r="AF12" s="11"/>
+      <c r="AD12" s="30"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="7"/>
     </row>
     <row r="13" spans="1:32" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="8"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="26"/>
-      <c r="V13" s="26"/>
-      <c r="W13" s="27"/>
-      <c r="AF13" s="11"/>
-    </row>
-    <row r="14" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
+      <c r="A13" s="16"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="14"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="45"/>
+      <c r="AF13" s="7"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
         <v>3</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="15">
         <f t="shared" ref="C14:M14" si="5">COUNTA(C15:C16)</f>
         <v>2</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H14" s="15">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L14" s="37">
+      <c r="L14" s="15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M14" s="37">
+      <c r="M14" s="15">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="O14" s="42" t="s">
+      <c r="O14" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="43" t="s">
+      <c r="P14" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="43" t="s">
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="U14" s="44"/>
-      <c r="V14" s="44"/>
-      <c r="W14" s="45"/>
-      <c r="AF14" s="11"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="33"/>
+      <c r="AF14" s="7"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I15" s="59"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="O15" s="46"/>
-      <c r="P15" s="47">
+      <c r="C15" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="O15" s="47"/>
+      <c r="P15" s="50">
         <f>COUNTA(C6,C11,C15,C21,C24,C20,C41,C43,C37,C35,C28,C49)</f>
         <v>11</v>
       </c>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="47">
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="52"/>
+      <c r="T15" s="50">
         <f>COUNTA(D5,D11,D16,D19,D24,D22,D42,D43,D44,D33,D34,D36,D37,D27,D28,D30,D48,D49)</f>
         <v>0</v>
       </c>
-      <c r="U15" s="48"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="49"/>
-      <c r="AF15" s="11"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="52"/>
+      <c r="AF15" s="7"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="O16" s="46"/>
-      <c r="P16" s="50"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="52"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="51"/>
-      <c r="W16" s="52"/>
+      <c r="C16" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="O16" s="47"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="54"/>
+      <c r="V16" s="54"/>
+      <c r="W16" s="55"/>
     </row>
     <row r="17" spans="1:23" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="50"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="50"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="52"/>
-    </row>
-    <row r="18" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="35">
+      <c r="A17" s="16"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="14"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="55"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
         <v>4</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="15">
         <f t="shared" ref="C18:M18" si="6">COUNTA(C19:C24)</f>
         <v>6</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="15">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="15">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="15">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G18" s="37">
+      <c r="G18" s="15">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="15">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="I18" s="37">
+      <c r="I18" s="15">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="J18" s="37">
+      <c r="J18" s="15">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K18" s="37">
+      <c r="K18" s="15">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="L18" s="37">
+      <c r="L18" s="15">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="M18" s="37">
+      <c r="M18" s="15">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="O18" s="46"/>
-      <c r="P18" s="50"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="50"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="52"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="53"/>
+      <c r="U18" s="54"/>
+      <c r="V18" s="54"/>
+      <c r="W18" s="55"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="39" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="O19" s="53"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="55"/>
-      <c r="R19" s="55"/>
-      <c r="S19" s="56"/>
-      <c r="T19" s="54"/>
-      <c r="U19" s="55"/>
-      <c r="V19" s="55"/>
-      <c r="W19" s="56"/>
+      <c r="C19" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="O19" s="48"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="57"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="56"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="58"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="39" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40" t="s">
+      <c r="C20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="24"/>
+      <c r="B21" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40" t="s">
+      <c r="C21" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="39" t="s">
+      <c r="A22" s="24"/>
+      <c r="B22" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22" s="58"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="M22" s="40"/>
+      <c r="C22" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M22" s="10"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="39" t="s">
+      <c r="A23" s="24"/>
+      <c r="B23" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" s="58"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40" t="s">
+      <c r="C23" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="39" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I24" s="59"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
+      <c r="C24" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="8"/>
-    </row>
-    <row r="26" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="35">
+      <c r="A25" s="16"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="23">
         <v>5</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="15">
         <f t="shared" ref="C26:M26" si="7">COUNTA(C27:C30)</f>
         <v>4</v>
       </c>
-      <c r="D26" s="37">
+      <c r="D26" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="E26" s="37">
+      <c r="E26" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G26" s="37">
+      <c r="G26" s="15">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="H26" s="37">
+      <c r="H26" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I26" s="37">
+      <c r="I26" s="15">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="J26" s="37">
+      <c r="J26" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K26" s="37">
+      <c r="K26" s="15">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="L26" s="37">
+      <c r="L26" s="15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M26" s="37">
+      <c r="M26" s="15">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="39" t="s">
+      <c r="A27" s="24"/>
+      <c r="B27" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="L27" s="40"/>
-      <c r="M27" s="40"/>
+      <c r="C27" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="39" t="s">
+      <c r="A28" s="24"/>
+      <c r="B28" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D28" s="58"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40" t="s">
+      <c r="C28" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="39" t="s">
+      <c r="A29" s="24"/>
+      <c r="B29" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="58"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40" t="s">
+      <c r="C29" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="B30" s="39" t="s">
+      <c r="A30" s="25"/>
+      <c r="B30" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D30" s="58"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
+      <c r="C30" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="8"/>
-    </row>
-    <row r="32" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="35">
+      <c r="A31" s="16"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
         <v>6</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="15">
         <f t="shared" ref="C32:M32" si="8">COUNTA(C33:C37)</f>
         <v>4</v>
       </c>
-      <c r="D32" s="37">
+      <c r="D32" s="15">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E32" s="37">
+      <c r="E32" s="15">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="F32" s="37">
+      <c r="F32" s="15">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="G32" s="37">
+      <c r="G32" s="15">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="H32" s="37">
+      <c r="H32" s="15">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="I32" s="37">
+      <c r="I32" s="15">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J32" s="37">
+      <c r="J32" s="15">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="K32" s="37">
+      <c r="K32" s="15">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="L32" s="37">
+      <c r="L32" s="15">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="M32" s="37">
+      <c r="M32" s="15">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
-      <c r="B33" s="39" t="s">
+      <c r="A33" s="24"/>
+      <c r="B33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33" s="58"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I33" s="59"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
+      <c r="C33" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I33" s="6"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="39" t="s">
+      <c r="A34" s="24"/>
+      <c r="B34" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D34" s="58"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="H34" s="59"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="M34" s="40"/>
+      <c r="C34" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M34" s="10"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
-      <c r="B35" s="39" t="s">
+      <c r="A35" s="24"/>
+      <c r="B35" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="K35" s="40"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="40"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
-      <c r="B36" s="39" t="s">
+      <c r="A36" s="24"/>
+      <c r="B36" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" s="58"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="I36" s="59"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="M36" s="40"/>
+      <c r="C36" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="9"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M36" s="10"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="39" t="s">
+      <c r="A37" s="25"/>
+      <c r="B37" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="58"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="L37" s="40"/>
-      <c r="M37" s="40"/>
+      <c r="C37" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="8"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="35">
+      <c r="A38" s="16"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="14"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="23">
         <v>7</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="15">
         <f t="shared" ref="C39:M39" si="9">COUNTA(C40:C44)</f>
         <v>5</v>
       </c>
-      <c r="D39" s="37">
+      <c r="D39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E39" s="37">
+      <c r="E39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F39" s="37">
+      <c r="F39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G39" s="37">
+      <c r="G39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H39" s="37">
+      <c r="H39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I39" s="37">
+      <c r="I39" s="15">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="J39" s="37">
+      <c r="J39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K39" s="37">
+      <c r="K39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L39" s="37">
+      <c r="L39" s="15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="M39" s="37">
+      <c r="M39" s="15">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
-      <c r="B40" s="39" t="s">
+      <c r="A40" s="24"/>
+      <c r="B40" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40" s="58"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40" t="s">
+      <c r="C40" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
-      <c r="B41" s="39" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41" s="58"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40" t="s">
+      <c r="C41" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
-      <c r="B42" s="39" t="s">
+      <c r="A42" s="24"/>
+      <c r="B42" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="40" t="s">
+      <c r="C42" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="9"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
-      <c r="B43" s="39" t="s">
+      <c r="A43" s="24"/>
+      <c r="B43" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40" t="s">
+      <c r="C43" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="39" t="s">
+      <c r="A44" s="25"/>
+      <c r="B44" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="58"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40" t="s">
+      <c r="C44" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="9"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="8"/>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="35">
+      <c r="A45" s="16"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="23">
         <v>8</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="37">
+      <c r="C46" s="15">
         <f t="shared" ref="C46:M46" si="10">COUNTA(C47:C49)</f>
         <v>3</v>
       </c>
-      <c r="D46" s="37">
+      <c r="D46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="E46" s="37">
+      <c r="E46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F46" s="37">
+      <c r="F46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G46" s="37">
+      <c r="G46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H46" s="37">
+      <c r="H46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I46" s="37">
+      <c r="I46" s="15">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="J46" s="37">
+      <c r="J46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K46" s="37">
+      <c r="K46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="L46" s="37">
+      <c r="L46" s="15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M46" s="37">
+      <c r="M46" s="15">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="38"/>
-      <c r="B47" s="39" t="s">
+      <c r="A47" s="24"/>
+      <c r="B47" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D47" s="58"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
-      <c r="M47" s="40" t="s">
+      <c r="C47" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="38"/>
-      <c r="B48" s="39" t="s">
+      <c r="A48" s="24"/>
+      <c r="B48" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D48" s="58"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="40" t="s">
+      <c r="C48" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="9"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="34"/>
-      <c r="B49" s="39" t="s">
+      <c r="A49" s="25"/>
+      <c r="B49" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="58" t="s">
-        <v>132</v>
-      </c>
-      <c r="D49" s="58"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-      <c r="H49" s="59"/>
-      <c r="I49" s="59" t="s">
-        <v>132</v>
-      </c>
-      <c r="J49" s="40"/>
-      <c r="K49" s="40"/>
-      <c r="L49" s="40"/>
-      <c r="M49" s="40" t="s">
+      <c r="C49" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>